<commit_message>
Refactor chart axis label alignment.
Issue #186
</commit_message>
<xml_diff>
--- a/test/functional/xlsx_files/chart_axis42.xlsx
+++ b/test/functional/xlsx_files/chart_axis42.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="16095" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -148,68 +148,32 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="43704320"/>
-        <c:axId val="43706624"/>
+        <c:axId val="61296640"/>
+        <c:axId val="61298560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="43704320"/>
+        <c:axId val="61296640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>XXX</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43706624"/>
+        <c:crossAx val="61298560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="r"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43706624"/>
+        <c:axId val="61298560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>YYY</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="43704320"/>
+        <c:crossAx val="61296640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>